<commit_message>
Se omitió la ventana modal de confirmación para realizar el cierre de dia
</commit_message>
<xml_diff>
--- a/assets/xls/register.xlsx
+++ b/assets/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Factura</t>
+          <t>Recibo</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SETP0000001</t>
+          <t>000068</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>17/10/2024 16:48:00</t>
+          <t>04/11/2024 16:43:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>17/10/2024 16:48:00</t>
+          <t>04/11/2024 16:51:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -508,6 +508,42 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>000069</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BBB01</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>04/11/2024 16:44:00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>04/11/2024 16:52:00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
         <v>1500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se modificaron los recibos y factura para mostrar nombres de parqueaderos mas largos
</commit_message>
<xml_diff>
--- a/assets/xls/register.xlsx
+++ b/assets/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000068</t>
+          <t>000076</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>04/11/2024 16:43:00</t>
+          <t>04/11/2024 17:57:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>04/11/2024 16:51:00</t>
+          <t>05/11/2024 10:25:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -502,19 +502,19 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1500</v>
+        <v>7000</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1500</v>
+        <v>14000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000069</t>
+          <t>000077</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -524,12 +524,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>04/11/2024 16:44:00</t>
+          <t>04/11/2024 17:58:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>04/11/2024 16:52:00</t>
+          <t>05/11/2024 10:34:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -538,13 +538,265 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1500</v>
+        <v>7000</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>1500</v>
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>000078</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CCC01</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>04/11/2024 17:58:00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>05/11/2024 10:34:00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>000079</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>DDD01</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>04/11/2024 17:58:00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>05/11/2024 10:35:00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>000080</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>EEE01</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>04/11/2024 17:58:00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>05/11/2024 10:35:00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>000081</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>FFF01</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>04/11/2024 17:59:00</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>05/11/2024 10:35:00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>000082</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>GGG01</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>04/11/2024 17:59:00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>05/11/2024 10:35:00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>000083</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>HHH01</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>04/11/2024 17:59:00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>05/11/2024 10:35:00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>000084</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>III01</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>04/11/2024 17:59:00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>05/11/2024 10:35:00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>14000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregó la columna tiempo a la tabla en cuadre de caja
</commit_message>
<xml_diff>
--- a/assets/xls/register.xlsx
+++ b/assets/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000076</t>
+          <t>000001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>04/11/2024 17:57:00</t>
+          <t>11/11/2024 10:20:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>05/11/2024 10:25:00</t>
+          <t>11/11/2024 10:21:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -502,19 +502,19 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>7000</v>
+        <v>1500</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>14000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000077</t>
+          <t>000002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -524,12 +524,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>04/11/2024 17:58:00</t>
+          <t>11/11/2024 10:20:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>05/11/2024 10:34:00</t>
+          <t>11/11/2024 10:25:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -538,34 +538,34 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>7000</v>
+        <v>1500</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>14000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>000078</t>
+          <t>000003</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CCC01</t>
+          <t>AAA01</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>04/11/2024 17:58:00</t>
+          <t>11/11/2024 10:23:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>05/11/2024 10:34:00</t>
+          <t>11/11/2024 10:25:00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -574,34 +574,34 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>7000</v>
+        <v>1500</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>14000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>000079</t>
+          <t>000004</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DDD01</t>
+          <t>BBB01</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>04/11/2024 17:58:00</t>
+          <t>11/11/2024 10:27:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>05/11/2024 10:35:00</t>
+          <t>11/11/2024 10:28:00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -610,34 +610,34 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>7000</v>
+        <v>1500</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>14000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>000080</t>
+          <t>000005</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EEE01</t>
+          <t>CCC01</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>04/11/2024 17:58:00</t>
+          <t>11/11/2024 10:30:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>05/11/2024 10:35:00</t>
+          <t>11/11/2024 10:31:00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -646,34 +646,34 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>7000</v>
+        <v>1500</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>14000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>000081</t>
+          <t>000006</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FFF01</t>
+          <t>DDD01</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>04/11/2024 17:59:00</t>
+          <t>11/11/2024 10:44:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>05/11/2024 10:35:00</t>
+          <t>11/11/2024 10:45:00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -682,34 +682,34 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>7000</v>
+        <v>1500</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>14000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>000082</t>
+          <t>000007</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>GGG01</t>
+          <t>AAA01</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>04/11/2024 17:59:00</t>
+          <t>11/11/2024 11:09:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>05/11/2024 10:35:00</t>
+          <t>11/11/2024 11:10:00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -718,34 +718,34 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>7000</v>
+        <v>1500</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>14000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>000083</t>
+          <t>000008</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>HHH01</t>
+          <t>BBB01</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>04/11/2024 17:59:00</t>
+          <t>10/11/2024 10:00:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>05/11/2024 10:35:00</t>
+          <t>11/11/2024 12:36:00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -756,47 +756,13 @@
       <c r="F9" t="n">
         <v>7000</v>
       </c>
-      <c r="G9" t="n">
-        <v>0</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>26:36</t>
+        </is>
       </c>
       <c r="H9" t="n">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>000084</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>III01</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>04/11/2024 17:59:00</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>05/11/2024 10:35:00</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>7000</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>14000</v>
+        <v>18500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se implementó ocultar y mostrar dinámicamente el menú web
</commit_message>
<xml_diff>
--- a/assets/xls/register.xlsx
+++ b/assets/xls/register.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Recibo</t>
+          <t>Factura</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>TEMP0000049</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>11/11/2024 10:20:00</t>
+          <t>27/11/2024 17:15:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11/11/2024 10:21:00</t>
+          <t>27/11/2024 17:17:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -504,8 +504,10 @@
       <c r="F2" t="n">
         <v>1500</v>
       </c>
-      <c r="G2" t="n">
-        <v>0</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>00:02</t>
+        </is>
       </c>
       <c r="H2" t="n">
         <v>1500</v>
@@ -514,58 +516,60 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000002</t>
+          <t>TEMP0000050</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BBB01</t>
+          <t>BBB001</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11/11/2024 10:20:00</t>
+          <t>27/11/2024 17:16:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>11/11/2024 10:25:00</t>
+          <t>27/11/2024 17:17:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Moto</t>
+          <t>Carro</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
+        <v>4000</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>00:01</t>
+        </is>
       </c>
       <c r="H3" t="n">
-        <v>1500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>000003</t>
+          <t>TEMP0000051</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AAA01</t>
+          <t>CCC01</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>11/11/2024 10:23:00</t>
+          <t>28/11/2024 09:45:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>11/11/2024 10:25:00</t>
+          <t>28/11/2024 09:46:00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -576,8 +580,10 @@
       <c r="F4" t="n">
         <v>1500</v>
       </c>
-      <c r="G4" t="n">
-        <v>0</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>00:01</t>
+        </is>
       </c>
       <c r="H4" t="n">
         <v>1500</v>
@@ -586,58 +592,60 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>000004</t>
+          <t>TEMP0000052</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BBB01</t>
+          <t>BBB002</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>11/11/2024 10:27:00</t>
+          <t>28/11/2024 09:45:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>11/11/2024 10:28:00</t>
+          <t>28/11/2024 09:46:00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Moto</t>
+          <t>Carro</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
+        <v>4000</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>00:01</t>
+        </is>
       </c>
       <c r="H5" t="n">
-        <v>1500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>000005</t>
+          <t>TEMP0000053</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CCC01</t>
+          <t>DDD01</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>11/11/2024 10:30:00</t>
+          <t>28/11/2024 09:47:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>11/11/2024 10:31:00</t>
+          <t>28/11/2024 09:47:00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -648,8 +656,10 @@
       <c r="F6" t="n">
         <v>1500</v>
       </c>
-      <c r="G6" t="n">
-        <v>0</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
       </c>
       <c r="H6" t="n">
         <v>1500</v>
@@ -658,22 +668,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>000006</t>
+          <t>TEMP0000054</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DDD01</t>
+          <t>AAA03</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>11/11/2024 10:44:00</t>
+          <t>28/11/2024 10:00:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>11/11/2024 10:45:00</t>
+          <t>28/11/2024 10:01:00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -684,8 +694,10 @@
       <c r="F7" t="n">
         <v>1500</v>
       </c>
-      <c r="G7" t="n">
-        <v>0</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>00:01</t>
+        </is>
       </c>
       <c r="H7" t="n">
         <v>1500</v>
@@ -694,58 +706,60 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>000007</t>
+          <t>TEMP0000055</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AAA01</t>
+          <t>EEE003</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>11/11/2024 11:09:00</t>
+          <t>28/11/2024 10:00:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>11/11/2024 11:10:00</t>
+          <t>28/11/2024 10:02:00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Moto</t>
+          <t>Carro</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
+        <v>4000</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>00:02</t>
+        </is>
       </c>
       <c r="H8" t="n">
-        <v>1500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>000008</t>
+          <t>TEMP0000056</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BBB01</t>
+          <t>FFF01</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10/11/2024 10:00:00</t>
+          <t>28/11/2024 11:19:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>11/11/2024 12:36:00</t>
+          <t>28/11/2024 11:20:00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -754,15 +768,15 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>7000</v>
+        <v>1500</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>26:36</t>
+          <t>00:01</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>18500</v>
+        <v>1500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se arregló el método page_resize en registro y cierre de día
</commit_message>
<xml_diff>
--- a/assets/xls/register.xlsx
+++ b/assets/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TEMP0000049</t>
+          <t>FETP0000001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>27/11/2024 17:15:00</t>
+          <t>03/12/2024 15:24:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>27/11/2024 17:17:00</t>
+          <t>03/12/2024 15:27:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>00:02</t>
+          <t>00:03</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -516,7 +516,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TEMP0000050</t>
+          <t>FETP0000002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -526,12 +526,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>27/11/2024 17:16:00</t>
+          <t>03/12/2024 15:25:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>27/11/2024 17:17:00</t>
+          <t>03/12/2024 15:27:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -544,239 +544,11 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>00:01</t>
+          <t>00:02</t>
         </is>
       </c>
       <c r="H3" t="n">
         <v>4000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>TEMP0000051</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>CCC01</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>28/11/2024 09:45:00</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>28/11/2024 09:46:00</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>00:01</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>TEMP0000052</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>BBB002</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>28/11/2024 09:45:00</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>28/11/2024 09:46:00</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Carro</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>4000</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>00:01</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>TEMP0000053</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>DDD01</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>28/11/2024 09:47:00</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>28/11/2024 09:47:00</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>00:00</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>TEMP0000054</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>AAA03</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>28/11/2024 10:00:00</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>28/11/2024 10:01:00</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>00:01</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>TEMP0000055</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>EEE003</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>28/11/2024 10:00:00</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>28/11/2024 10:02:00</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Carro</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>4000</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>00:02</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>TEMP0000056</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>FFF01</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>28/11/2024 11:19:00</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>28/11/2024 11:20:00</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>00:01</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>1500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se arregló el cierre de día y se agregó el vehiculo y el usuario que atendió al cliente en los recibos
</commit_message>
<xml_diff>
--- a/assets/xls/register.xlsx
+++ b/assets/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FETP0000001</t>
+          <t>FEP0000001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>03/12/2024 15:24:00</t>
+          <t>27/01/2025 11:22:45</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>03/12/2024 15:27:00</t>
+          <t>27/01/2025 11:24:27</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>00:03</t>
+          <t>00:01:01</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -516,7 +516,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FETP0000002</t>
+          <t>FEP0000002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -526,12 +526,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>03/12/2024 15:25:00</t>
+          <t>27/01/2025 09:23:12</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>03/12/2024 15:27:00</t>
+          <t>27/01/2025 11:24:46</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -544,11 +544,49 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>00:02</t>
+          <t>02:01:01</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>4000</v>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FEP0000003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CCC01</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>26/01/2025 23:26:22</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>27/01/2025 11:28:02</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Moto</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>12:01:01</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>7750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se reorganizaron los recibos y factura y se acgregaron los campos atendido por, duplicado por y valor del duplicado
</commit_message>
<xml_diff>
--- a/assets/xls/register.xlsx
+++ b/assets/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>27/01/2025 11:22:45</t>
+          <t>28/01/2025 09:29:40</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>27/01/2025 11:24:27</t>
+          <t>28/01/2025 09:36:20</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>00:01:01</t>
+          <t>00:06:06</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -526,12 +526,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>27/01/2025 09:23:12</t>
+          <t>28/01/2025 09:35:45</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>27/01/2025 11:24:46</t>
+          <t>28/01/2025 09:36:49</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -544,49 +544,11 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>02:01:01</t>
+          <t>00:01:01</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>FEP0000003</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>CCC01</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>26/01/2025 23:26:22</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>27/01/2025 11:28:02</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Moto</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>7000</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>12:01:01</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>7750</v>
+        <v>4000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualizaron los datos de configuración en cuadre de caja y cierre de dia
</commit_message>
<xml_diff>
--- a/assets/xls/register.xlsx
+++ b/assets/xls/register.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FEP0000001</t>
+          <t>FEP0000003</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>28/01/2025 09:29:40</t>
+          <t>01/02/2025 10:08:08</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>28/01/2025 09:36:20</t>
+          <t>01/02/2025 10:10:14</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -506,49 +506,11 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>00:06:06</t>
+          <t>00:02:02</t>
         </is>
       </c>
       <c r="H2" t="n">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>FEP0000002</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>BBB001</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>28/01/2025 09:35:45</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>28/01/2025 09:36:49</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Carro</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>4000</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>00:01:01</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>4000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>